<commit_message>
Removed duplicate entries after Johan's e-mail
</commit_message>
<xml_diff>
--- a/Documentation/Shopping List_modified_v04.xlsx
+++ b/Documentation/Shopping List_modified_v04.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="200" windowWidth="31900" windowHeight="21040"/>
+    <workbookView xWindow="7080" yWindow="0" windowWidth="31900" windowHeight="21040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="135">
   <si>
     <t>Item</t>
   </si>
@@ -346,15 +346,6 @@
     <t>Pick up Solna and pay by team</t>
   </si>
   <si>
-    <t>Connection Cables</t>
-  </si>
-  <si>
-    <t>Ultrasound Sensor Maxbotix HRLV-EZ4</t>
-  </si>
-  <si>
-    <t>RVVP 4x0.2 skärmad svart</t>
-  </si>
-  <si>
     <t>http://www.electrokit.com/testsladdar-med-krokodilklammor-30mm-50cm-10pack.44765</t>
   </si>
   <si>
@@ -367,15 +358,9 @@
     <t>no</t>
   </si>
   <si>
-    <t>Banan plugs</t>
-  </si>
-  <si>
     <t>http://www.kjell.com/se/sortiment/el/batterier/specialbatteri-blockbatteri/varta-6-v-batteri-%284r25%29-p32144</t>
   </si>
   <si>
-    <t>http://www.kjell.com/se/sortiment/el/verktyg/matinstrument/matsladdar-prober-kontakter/labbkontakter-4-mm/4-mm-labbpropp-39-mm-svart-p37872</t>
-  </si>
-  <si>
     <t>https://www.elfa.se/sv/usb-kablage-usb-ttl-cmos-ftdi-ttl-232r-3v3/p/17320674?q=*&amp;filter_Buyable=1&amp;filter_Category7=USB-kablage+med+FT232RQ&amp;filter_Category3=Linj%C3%A4ra+kretsar&amp;filter_Category4=Gr%C3%A4nssnittskretsar&amp;filter_Category6=USB-moduler+med+FT232&amp;filter_Category5=Interface-kretsar&amp;page=2&amp;origPageSize=50&amp;simi=99.5</t>
   </si>
   <si>
@@ -391,12 +376,6 @@
     <t>Electrokit crocodile connectors</t>
   </si>
   <si>
-    <t>Electrokit distance ultrasound meter</t>
-  </si>
-  <si>
-    <t>Electrokit cable 1m</t>
-  </si>
-  <si>
     <t>Electrokit shipping cost</t>
   </si>
   <si>
@@ -409,9 +388,6 @@
     <t>Elfa Screws Nylon M3 30mm</t>
   </si>
   <si>
-    <t>Elfa Contact hus 5P</t>
-  </si>
-  <si>
     <t>Actual cost (how much was actually paid *)</t>
   </si>
   <si>
@@ -427,18 +403,6 @@
     <t>Elfa Nuts Nylon M3</t>
   </si>
   <si>
-    <t>Elfa USB2FTDI3V3</t>
-  </si>
-  <si>
-    <t>Elfa USB2FTDI5V</t>
-  </si>
-  <si>
-    <t>Elfa Connector DF13-5S-1.25C</t>
-  </si>
-  <si>
-    <t>Elfa USB cable</t>
-  </si>
-  <si>
     <t xml:space="preserve">YES </t>
   </si>
   <si>
@@ -496,7 +460,19 @@
     <t>http://www.kjell.com/se/sortiment/el/verktyg/matinstrument/matsladdar-prober-kontakter/labbkontakter-4-mm/4-mm-labbpropp-55-mm-svart-p37877</t>
   </si>
   <si>
-    <t>Red is what Vlasios cannot find in receipts or cannot be justified (e.g. Sharan lost a receipt but I know it) This may mean that the team intented to buy but did not buy these items in the end ?</t>
+    <t>Elfa Contact hus 5P Connector DF13-5S-1.25C</t>
+  </si>
+  <si>
+    <t>Electrokit Ultrasound Sensor Maxbotix HRLV-EZ4</t>
+  </si>
+  <si>
+    <t>Electrokit cable 1m RVVP 4x0.2 skärmad svart</t>
+  </si>
+  <si>
+    <t>Elfa USB cable USB2FTDI5V</t>
+  </si>
+  <si>
+    <t>Elfa USB cable  USB2FTDI3V3</t>
   </si>
 </sst>
 </file>
@@ -558,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,12 +544,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -808,8 +778,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -874,22 +874,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -945,6 +939,21 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1000,6 +1009,21 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1270,7 +1294,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1278,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T71"/>
+  <dimension ref="A2:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1361,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>2</v>
@@ -1527,7 +1551,7 @@
         <v>89.99</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D63" si="0">B11*C11</f>
+        <f t="shared" ref="D11:D42" si="0">B11*C11</f>
         <v>179.98</v>
       </c>
       <c r="E11" s="2">
@@ -1546,7 +1570,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="14">
-        <f t="shared" ref="J11:J63" si="1">F11*H11</f>
+        <f t="shared" ref="J11:J42" si="1">F11*H11</f>
         <v>1920.316032</v>
       </c>
       <c r="K11" s="14">
@@ -1593,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F63" si="2">D12+E12</f>
+        <f t="shared" ref="F12:F42" si="2">D12+E12</f>
         <v>3180</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1856,306 +1880,281 @@
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="22">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E19" s="2">
-        <v>49</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="2"/>
-        <v>78</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="14">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
+      <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="10" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="22">
-        <v>369</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>369</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="2"/>
-        <v>369</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="14">
-        <f t="shared" si="1"/>
-        <v>369</v>
-      </c>
+      <c r="A20" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="10" t="s">
+      <c r="M20" s="12"/>
+      <c r="N20" s="13"/>
+      <c r="R20" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2</v>
-      </c>
-      <c r="C21" s="22">
-        <v>9.3800000000000008</v>
+      <c r="A21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2"/>
+      <c r="H21" s="12">
+        <v>1</v>
+      </c>
+      <c r="I21" s="12"/>
       <c r="J21" s="14">
-        <f t="shared" si="1"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="10" t="s">
-        <v>98</v>
+        <v>149</v>
+      </c>
+      <c r="K21" s="14">
+        <v>149</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" s="12"/>
+      <c r="N21" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="22"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="13"/>
-      <c r="R23" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="12">
-        <v>1</v>
-      </c>
-      <c r="C24" s="12">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="14">
-        <v>149</v>
-      </c>
-      <c r="K24" s="14">
-        <v>149</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B26" s="12">
-        <v>1</v>
-      </c>
-      <c r="C26" s="12">
+        <v>117</v>
+      </c>
+      <c r="B23" s="12">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12">
         <v>59.9</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>59.9</v>
       </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
         <f t="shared" si="2"/>
         <v>59.9</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="12">
-        <v>1</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="14">
+      <c r="H23" s="12">
+        <v>1</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="14">
         <f t="shared" si="1"/>
         <v>59.9</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K23" s="14">
         <v>59.9</v>
       </c>
-      <c r="L26" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M26" s="12"/>
-      <c r="N26" s="13" t="s">
+      <c r="L23" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="13"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B28" s="12">
-        <v>1</v>
-      </c>
-      <c r="C28" s="12">
+    <row r="24" spans="1:20">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
         <v>29.9</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>29.9</v>
       </c>
-      <c r="E28" s="12">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
         <f t="shared" si="2"/>
         <v>29.9</v>
       </c>
+      <c r="G25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="14">
+        <f t="shared" si="1"/>
+        <v>29.9</v>
+      </c>
+      <c r="K25" s="14">
+        <v>29.9</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="20"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="12">
+        <v>10</v>
+      </c>
+      <c r="C27" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="D27" s="2">
+        <f>B27*C27</f>
+        <v>29</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27:F28" si="3">D27+E27</f>
+        <v>29</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="12">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14">
+        <f t="shared" ref="J27:J28" si="4">F27*H27</f>
+        <v>29</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
+      <c r="C28" s="21">
+        <v>369</v>
+      </c>
+      <c r="D28" s="2">
+        <f>B28*C28</f>
+        <v>369</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="3"/>
+        <v>369</v>
+      </c>
       <c r="G28" s="12" t="s">
         <v>19</v>
       </c>
@@ -2164,54 +2163,84 @@
       </c>
       <c r="I28" s="12"/>
       <c r="J28" s="14">
-        <f t="shared" si="1"/>
-        <v>29.9</v>
-      </c>
-      <c r="K28" s="14">
-        <v>29.9</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>369</v>
+      </c>
+      <c r="K28" s="14"/>
       <c r="L28" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="15"/>
+        <v>103</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="A29" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1</v>
+      </c>
+      <c r="C29" s="21">
+        <v>9.375</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" ref="D29" si="5">B29*C29</f>
+        <v>9.375</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <f>D29+E29</f>
+        <v>9.375</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="12">
+        <v>1</v>
+      </c>
       <c r="I29" s="12"/>
-      <c r="J29" s="14"/>
+      <c r="J29" s="14">
+        <f>F29*H29</f>
+        <v>9.375</v>
+      </c>
       <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="20"/>
+      <c r="L29" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="26" t="s">
-        <v>106</v>
+      <c r="A30" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="B30" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C30" s="21">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
         <f>B30*C30</f>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E30" s="12">
-        <v>0</v>
+        <v>63.2</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" ref="F30:F31" si="3">D30+E30</f>
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>19</v>
@@ -2221,75 +2250,52 @@
       </c>
       <c r="I30" s="12"/>
       <c r="J30" s="14">
-        <f t="shared" ref="J30:J31" si="4">F30*H30</f>
-        <v>29</v>
+        <f>F30*H30</f>
+        <v>79</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="12">
-        <v>1</v>
-      </c>
-      <c r="C31" s="21">
-        <v>369</v>
-      </c>
-      <c r="D31" s="2">
-        <f>B31*C31</f>
-        <v>369</v>
-      </c>
-      <c r="E31" s="12">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="3"/>
-        <v>369</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="12">
-        <v>1</v>
-      </c>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="14">
-        <f t="shared" si="4"/>
-        <v>369</v>
-      </c>
+      <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="14" t="s">
-        <v>110</v>
-      </c>
+      <c r="L31" s="14"/>
       <c r="M31" s="12"/>
       <c r="N31" s="20"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B32" s="12">
-        <v>1</v>
-      </c>
-      <c r="C32" s="21">
-        <v>9.375</v>
+        <v>3</v>
+      </c>
+      <c r="C32" s="12">
+        <v>10.925000000000001</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32" si="5">B32*C32</f>
-        <v>9.375</v>
+        <f>B32*C32</f>
+        <v>32.775000000000006</v>
       </c>
       <c r="E32" s="12">
         <v>0</v>
       </c>
       <c r="F32" s="2">
         <f>D32+E32</f>
-        <v>9.375</v>
+        <v>32.775000000000006</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>19</v>
@@ -2300,34 +2306,51 @@
       <c r="I32" s="12"/>
       <c r="J32" s="14">
         <f>F32*H32</f>
-        <v>9.375</v>
+        <v>32.775000000000006</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="M32" s="12"/>
-      <c r="N32" s="20"/>
+        <v>107</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O32" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q32" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="R32" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="26" t="s">
-        <v>109</v>
+      <c r="A33" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="B33" s="12">
-        <v>0</v>
-      </c>
-      <c r="C33" s="21">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C33" s="12">
+        <v>2.6120000000000001</v>
       </c>
       <c r="D33" s="2">
         <f>B33*C33</f>
-        <v>0</v>
+        <v>5.2240000000000002</v>
       </c>
       <c r="E33" s="12">
-        <v>63.2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="2">
-        <v>79</v>
+        <f>D33+E33</f>
+        <v>5.2240000000000002</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>19</v>
@@ -2338,51 +2361,106 @@
       <c r="I33" s="12"/>
       <c r="J33" s="14">
         <f>F33*H33</f>
-        <v>79</v>
+        <v>5.2240000000000002</v>
       </c>
       <c r="K33" s="14"/>
       <c r="L33" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="M33" s="12"/>
-      <c r="N33" s="20"/>
+        <v>107</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N33" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="A34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="12">
+        <v>3</v>
+      </c>
+      <c r="C34" s="12">
+        <v>10.925000000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <f>B34*C34</f>
+        <v>32.775000000000006</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <f>D34+E34</f>
+        <v>32.775000000000006</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="12">
+        <v>1</v>
+      </c>
       <c r="I34" s="12"/>
-      <c r="J34" s="14"/>
+      <c r="J34" s="14">
+        <f>F34*H34</f>
+        <v>32.775000000000006</v>
+      </c>
       <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="20"/>
+      <c r="L34" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O34" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P34" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q34" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="R34" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="11" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B35" s="12">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C35" s="12">
-        <v>10.925000000000001</v>
+        <v>1.3875</v>
       </c>
       <c r="D35" s="2">
-        <f>B35*C35</f>
-        <v>32.775000000000006</v>
+        <f t="shared" si="0"/>
+        <v>41.625</v>
       </c>
       <c r="E35" s="12">
         <v>0</v>
       </c>
       <c r="F35" s="2">
-        <f>D35+E35</f>
-        <v>32.775000000000006</v>
+        <f t="shared" si="2"/>
+        <v>41.625</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>19</v>
@@ -2392,15 +2470,15 @@
       </c>
       <c r="I35" s="12"/>
       <c r="J35" s="14">
-        <f>F35*H35</f>
-        <v>32.775000000000006</v>
+        <f t="shared" si="1"/>
+        <v>41.625</v>
       </c>
       <c r="K35" s="14"/>
       <c r="L35" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N35" s="20" t="s">
         <v>91</v>
@@ -2415,68 +2493,45 @@
         <v>90</v>
       </c>
       <c r="R35" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="12">
-        <v>2</v>
-      </c>
-      <c r="C36" s="12">
-        <v>2.6120000000000001</v>
-      </c>
-      <c r="D36" s="2">
-        <f>B36*C36</f>
-        <v>5.2240000000000002</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <f>D36+E36</f>
-        <v>5.2240000000000002</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="12">
-        <v>1</v>
-      </c>
+      <c r="A36" s="11"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="14">
-        <f>F36*H36</f>
-        <v>5.2240000000000002</v>
-      </c>
+      <c r="J36" s="14"/>
       <c r="K36" s="14"/>
-      <c r="L36" s="14" t="s">
-        <v>115</v>
-      </c>
+      <c r="L36" s="14"/>
       <c r="M36" s="12"/>
       <c r="N36" s="20"/>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="11" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B37" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="12">
-        <v>10.925000000000001</v>
+        <v>236.25</v>
       </c>
       <c r="D37" s="2">
-        <f>B37*C37</f>
-        <v>32.775000000000006</v>
+        <f t="shared" ref="D37" si="6">B37*C37</f>
+        <v>236.25</v>
       </c>
       <c r="E37" s="12">
         <v>0</v>
       </c>
       <c r="F37" s="2">
-        <f>D37+E37</f>
-        <v>32.775000000000006</v>
+        <f t="shared" ref="F37" si="7">D37+E37</f>
+        <v>236.25</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>19</v>
@@ -2486,15 +2541,15 @@
       </c>
       <c r="I37" s="12"/>
       <c r="J37" s="14">
-        <f>F37*H37</f>
-        <v>32.775000000000006</v>
+        <f t="shared" ref="J37" si="8">F37*H37</f>
+        <v>236.25</v>
       </c>
       <c r="K37" s="14"/>
       <c r="L37" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N37" s="20" t="s">
         <v>91</v>
@@ -2509,29 +2564,29 @@
         <v>90</v>
       </c>
       <c r="R37" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B38" s="12">
         <v>30</v>
       </c>
       <c r="C38" s="12">
-        <v>1.3875</v>
+        <v>0.83374999999999999</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="0"/>
-        <v>41.625</v>
+        <v>25.012499999999999</v>
       </c>
       <c r="E38" s="12">
         <v>0</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="2"/>
-        <v>41.625</v>
+        <v>25.012499999999999</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>19</v>
@@ -2542,14 +2597,14 @@
       <c r="I38" s="12"/>
       <c r="J38" s="14">
         <f t="shared" si="1"/>
-        <v>41.625</v>
+        <v>25.012499999999999</v>
       </c>
       <c r="K38" s="14"/>
       <c r="L38" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N38" s="20" t="s">
         <v>91</v>
@@ -2564,7 +2619,7 @@
         <v>90</v>
       </c>
       <c r="R38" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2585,24 +2640,24 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="11" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B40" s="12">
         <v>1</v>
       </c>
       <c r="C40" s="12">
-        <v>236.25</v>
+        <v>265</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" ref="D40" si="6">B40*C40</f>
-        <v>236.25</v>
+        <f t="shared" ref="D40" si="9">B40*C40</f>
+        <v>265</v>
       </c>
       <c r="E40" s="12">
         <v>0</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" ref="F40" si="7">D40+E40</f>
-        <v>236.25</v>
+        <f t="shared" ref="F40" si="10">D40+E40</f>
+        <v>265</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>19</v>
@@ -2612,15 +2667,15 @@
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="14">
-        <f t="shared" ref="J40" si="8">F40*H40</f>
-        <v>236.25</v>
+        <f t="shared" ref="J40" si="11">F40*H40</f>
+        <v>265</v>
       </c>
       <c r="K40" s="14"/>
       <c r="L40" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="N40" s="20" t="s">
         <v>91</v>
@@ -2635,100 +2690,86 @@
         <v>90</v>
       </c>
       <c r="R40" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="12">
-        <v>30</v>
-      </c>
-      <c r="C41" s="12">
-        <v>0.83374999999999999</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="20"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="12">
+        <v>2</v>
+      </c>
+      <c r="C42" s="21">
+        <v>49.9</v>
+      </c>
+      <c r="D42" s="2">
         <f t="shared" si="0"/>
-        <v>25.012499999999999</v>
-      </c>
-      <c r="E41" s="12">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2">
+        <v>99.8</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
         <f t="shared" si="2"/>
-        <v>25.012499999999999</v>
-      </c>
-      <c r="G41" s="12" t="s">
+        <v>99.8</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H41" s="12">
-        <v>1</v>
-      </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="14">
+      <c r="H42" s="12">
+        <v>1</v>
+      </c>
+      <c r="I42" s="12"/>
+      <c r="J42" s="14">
         <f t="shared" si="1"/>
-        <v>25.012499999999999</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="M41" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="N41" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O41" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q41" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="R41" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
-      <c r="A42" s="11"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="14"/>
+        <v>99.8</v>
+      </c>
       <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="12"/>
+      <c r="L42" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="N42" s="20"/>
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B43" s="12">
         <v>1</v>
       </c>
-      <c r="C43" s="12">
-        <v>265</v>
+      <c r="C43" s="21">
+        <v>22.9</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" ref="D43" si="9">B43*C43</f>
-        <v>265</v>
+        <f t="shared" ref="D43" si="12">B43*C43</f>
+        <v>22.9</v>
       </c>
       <c r="E43" s="12">
         <v>0</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" ref="F43" si="10">D43+E43</f>
-        <v>265</v>
+        <f t="shared" ref="F43" si="13">D43+E43</f>
+        <v>22.9</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>19</v>
@@ -2738,119 +2779,95 @@
       </c>
       <c r="I43" s="12"/>
       <c r="J43" s="14">
-        <f t="shared" ref="J43" si="11">F43*H43</f>
-        <v>265</v>
+        <f t="shared" ref="J43" si="14">F43*H43</f>
+        <v>22.9</v>
       </c>
       <c r="K43" s="14"/>
       <c r="L43" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="M43" s="12"/>
-      <c r="N43" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O43" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q43" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="R43" s="10" t="s">
-        <v>98</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N43" s="20"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="11"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
+      <c r="A44" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="21">
+        <v>22.9</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" ref="D44" si="15">B44*C44</f>
+        <v>22.9</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="shared" ref="F44" si="16">D44+E44</f>
+        <v>22.9</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="12">
+        <v>1</v>
+      </c>
       <c r="I44" s="12"/>
-      <c r="J44" s="14"/>
+      <c r="J44" s="14">
+        <f t="shared" ref="J44" si="17">F44*H44</f>
+        <v>22.9</v>
+      </c>
       <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="12"/>
+      <c r="L44" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="N44" s="20"/>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" s="12">
-        <v>1</v>
-      </c>
-      <c r="C45" s="12">
-        <v>212</v>
-      </c>
-      <c r="D45" s="2">
-        <f t="shared" si="0"/>
-        <v>212</v>
-      </c>
-      <c r="E45" s="12">
-        <v>0</v>
-      </c>
-      <c r="F45" s="2">
-        <f t="shared" si="2"/>
-        <v>212</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="12">
-        <v>1</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="12"/>
-      <c r="J45" s="14">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
+      <c r="J45" s="14"/>
       <c r="K45" s="14"/>
       <c r="L45" s="14"/>
-      <c r="M45" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="N45" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O45" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P45" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q45" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="R45" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="M45" s="12"/>
+      <c r="N45" s="20"/>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="24" t="s">
-        <v>120</v>
+      <c r="A46" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="B46" s="12">
-        <v>1</v>
-      </c>
-      <c r="C46" s="12">
-        <v>236.25</v>
+        <v>4</v>
+      </c>
+      <c r="C46" s="21">
+        <v>34.9</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="0"/>
-        <v>236.25</v>
+        <f t="shared" ref="D46" si="18">B46*C46</f>
+        <v>139.6</v>
       </c>
       <c r="E46" s="12">
         <v>0</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="2"/>
-        <v>236.25</v>
+        <f t="shared" ref="F46" si="19">D46+E46</f>
+        <v>139.6</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>19</v>
@@ -2860,119 +2877,91 @@
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="14">
-        <f t="shared" si="1"/>
-        <v>236.25</v>
+        <f t="shared" ref="J46" si="20">F46*H46</f>
+        <v>139.6</v>
       </c>
       <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="N46" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O46" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="L46" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M46" s="12"/>
+      <c r="N46" s="20"/>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B47" s="12">
-        <v>2</v>
-      </c>
-      <c r="C47" s="12">
-        <v>2.61</v>
-      </c>
-      <c r="D47" s="2">
-        <f t="shared" si="0"/>
-        <v>5.22</v>
-      </c>
-      <c r="E47" s="12">
-        <v>0</v>
-      </c>
-      <c r="F47" s="2">
-        <f t="shared" si="2"/>
-        <v>5.22</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="12">
-        <v>1</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
       <c r="I47" s="12"/>
-      <c r="J47" s="14">
-        <f t="shared" si="1"/>
-        <v>5.22</v>
-      </c>
+      <c r="J47" s="14"/>
       <c r="K47" s="14"/>
       <c r="L47" s="14"/>
-      <c r="M47" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N47" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O47" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="P47" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q47" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="R47" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="M47" s="12"/>
+      <c r="N47" s="20"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="11"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
+      <c r="A48" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C48" s="21">
+        <v>249</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" ref="D48" si="21">B48*C48</f>
+        <v>15.936</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" ref="F48" si="22">D48+E48</f>
+        <v>15.936</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="12">
+        <v>1</v>
+      </c>
       <c r="I48" s="12"/>
-      <c r="J48" s="14"/>
+      <c r="J48" s="14">
+        <f t="shared" ref="J48" si="23">F48*H48</f>
+        <v>15.936</v>
+      </c>
       <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
+      <c r="L48" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="M48" s="12"/>
       <c r="N48" s="20"/>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B49" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" s="21">
-        <v>49.9</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2">
-        <f t="shared" si="0"/>
-        <v>99.8</v>
+        <f t="shared" ref="D49" si="24">B49*C49</f>
+        <v>65</v>
       </c>
       <c r="E49" s="12">
         <v>0</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="2"/>
-        <v>99.8</v>
+        <f t="shared" ref="F49" si="25">D49+E49</f>
+        <v>65</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>19</v>
@@ -2982,38 +2971,36 @@
       </c>
       <c r="I49" s="12"/>
       <c r="J49" s="14">
-        <f t="shared" si="1"/>
-        <v>99.8</v>
+        <f t="shared" ref="J49" si="26">F49*H49</f>
+        <v>65</v>
       </c>
       <c r="K49" s="14"/>
       <c r="L49" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="M49" s="12" t="s">
-        <v>100</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="M49" s="12"/>
       <c r="N49" s="20"/>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B50" s="12">
         <v>1</v>
       </c>
       <c r="C50" s="21">
-        <v>22.9</v>
+        <v>19.95</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" ref="D50" si="12">B50*C50</f>
-        <v>22.9</v>
+        <f t="shared" ref="D50" si="27">B50*C50</f>
+        <v>19.95</v>
       </c>
       <c r="E50" s="12">
         <v>0</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" ref="F50" si="13">D50+E50</f>
-        <v>22.9</v>
+        <f t="shared" ref="F50" si="28">D50+E50</f>
+        <v>19.95</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>19</v>
@@ -3023,38 +3010,36 @@
       </c>
       <c r="I50" s="12"/>
       <c r="J50" s="14">
-        <f t="shared" ref="J50" si="14">F50*H50</f>
-        <v>22.9</v>
+        <f t="shared" ref="J50" si="29">F50*H50</f>
+        <v>19.95</v>
       </c>
       <c r="K50" s="14"/>
       <c r="L50" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="M50" s="12" t="s">
-        <v>140</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="M50" s="12"/>
       <c r="N50" s="20"/>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B51" s="12">
         <v>1</v>
       </c>
       <c r="C51" s="21">
-        <v>22.9</v>
+        <v>26</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" ref="D51" si="15">B51*C51</f>
-        <v>22.9</v>
+        <f t="shared" ref="D51" si="30">B51*C51</f>
+        <v>26</v>
       </c>
       <c r="E51" s="12">
         <v>0</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" ref="F51" si="16">D51+E51</f>
-        <v>22.9</v>
+        <f t="shared" ref="F51" si="31">D51+E51</f>
+        <v>26</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>19</v>
@@ -3064,469 +3049,194 @@
       </c>
       <c r="I51" s="12"/>
       <c r="J51" s="14">
-        <f t="shared" ref="J51" si="17">F51*H51</f>
-        <v>22.9</v>
+        <f t="shared" ref="J51" si="32">F51*H51</f>
+        <v>26</v>
       </c>
       <c r="K51" s="14"/>
       <c r="L51" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="M51" s="12" t="s">
-        <v>141</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="M51" s="12"/>
       <c r="N51" s="20"/>
     </row>
     <row r="52" spans="1:15">
-      <c r="A52" s="11"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
+      <c r="A52" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="12">
+        <v>1</v>
+      </c>
+      <c r="C52" s="21">
+        <v>3</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" ref="D52" si="33">B52*C52</f>
+        <v>3</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" ref="F52" si="34">D52+E52</f>
+        <v>3</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="12">
+        <v>1</v>
+      </c>
       <c r="I52" s="12"/>
-      <c r="J52" s="14"/>
+      <c r="J52" s="14">
+        <f t="shared" ref="J52" si="35">F52*H52</f>
+        <v>3</v>
+      </c>
       <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
+      <c r="L52" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="M52" s="12"/>
       <c r="N52" s="20"/>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B53" s="12">
-        <v>4</v>
-      </c>
-      <c r="C53" s="21">
-        <v>34.9</v>
-      </c>
-      <c r="D53" s="2">
-        <f t="shared" ref="D53" si="18">B53*C53</f>
-        <v>139.6</v>
-      </c>
-      <c r="E53" s="12">
-        <v>0</v>
-      </c>
-      <c r="F53" s="2">
-        <f t="shared" ref="F53" si="19">D53+E53</f>
-        <v>139.6</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="12">
-        <v>1</v>
-      </c>
+      <c r="A53" s="11"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
       <c r="I53" s="12"/>
-      <c r="J53" s="14">
-        <f t="shared" ref="J53" si="20">F53*H53</f>
-        <v>139.6</v>
-      </c>
+      <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="14" t="s">
-        <v>104</v>
-      </c>
+      <c r="L53" s="14"/>
       <c r="M53" s="12"/>
       <c r="N53" s="20"/>
     </row>
     <row r="54" spans="1:15">
-      <c r="A54" s="11"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
+      <c r="A54" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="12">
+        <v>1</v>
+      </c>
+      <c r="C54" s="21">
+        <v>29.9</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" ref="D54" si="36">B54*C54</f>
+        <v>29.9</v>
+      </c>
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2">
+        <f t="shared" ref="F54" si="37">D54+E54</f>
+        <v>29.9</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="12">
+        <v>1</v>
+      </c>
       <c r="I54" s="12"/>
-      <c r="J54" s="14"/>
+      <c r="J54" s="14">
+        <f t="shared" ref="J54" si="38">F54*H54</f>
+        <v>29.9</v>
+      </c>
       <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
+      <c r="L54" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="M54" s="12"/>
       <c r="N54" s="20"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="C55" s="21">
-        <v>249</v>
-      </c>
-      <c r="D55" s="2">
-        <f t="shared" ref="D55" si="21">B55*C55</f>
-        <v>15.936</v>
-      </c>
-      <c r="E55" s="12">
-        <v>0</v>
-      </c>
-      <c r="F55" s="2">
-        <f t="shared" ref="F55" si="22">D55+E55</f>
-        <v>15.936</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H55" s="12">
-        <v>1</v>
-      </c>
+      <c r="A55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
       <c r="I55" s="12"/>
-      <c r="J55" s="14">
-        <f t="shared" ref="J55" si="23">F55*H55</f>
-        <v>15.936</v>
-      </c>
+      <c r="J55" s="14"/>
       <c r="K55" s="14"/>
-      <c r="L55" s="14" t="s">
-        <v>138</v>
-      </c>
+      <c r="L55" s="14"/>
       <c r="M55" s="12"/>
       <c r="N55" s="20"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" s="12">
-        <v>1</v>
-      </c>
-      <c r="C56" s="21">
-        <v>65</v>
-      </c>
-      <c r="D56" s="2">
-        <f t="shared" ref="D56" si="24">B56*C56</f>
-        <v>65</v>
-      </c>
-      <c r="E56" s="12">
-        <v>0</v>
-      </c>
-      <c r="F56" s="2">
-        <f t="shared" ref="F56" si="25">D56+E56</f>
-        <v>65</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H56" s="12">
-        <v>1</v>
-      </c>
+      <c r="A56" s="11"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
       <c r="I56" s="12"/>
-      <c r="J56" s="14">
-        <f t="shared" ref="J56" si="26">F56*H56</f>
-        <v>65</v>
-      </c>
+      <c r="J56" s="14"/>
       <c r="K56" s="14"/>
-      <c r="L56" s="14" t="s">
-        <v>138</v>
-      </c>
+      <c r="L56" s="14"/>
       <c r="M56" s="12"/>
       <c r="N56" s="20"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B57" s="12">
-        <v>1</v>
-      </c>
-      <c r="C57" s="21">
-        <v>19.95</v>
-      </c>
-      <c r="D57" s="2">
-        <f t="shared" ref="D57" si="27">B57*C57</f>
-        <v>19.95</v>
-      </c>
-      <c r="E57" s="12">
-        <v>0</v>
-      </c>
-      <c r="F57" s="2">
-        <f t="shared" ref="F57" si="28">D57+E57</f>
-        <v>19.95</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H57" s="12">
-        <v>1</v>
-      </c>
+      <c r="A57" s="11"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
       <c r="I57" s="12"/>
-      <c r="J57" s="14">
-        <f t="shared" ref="J57" si="29">F57*H57</f>
-        <v>19.95</v>
-      </c>
+      <c r="J57" s="14"/>
       <c r="K57" s="14"/>
-      <c r="L57" s="14" t="s">
-        <v>138</v>
-      </c>
+      <c r="L57" s="14"/>
       <c r="M57" s="12"/>
-      <c r="N57" s="20"/>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B58" s="12">
-        <v>1</v>
-      </c>
-      <c r="C58" s="21">
-        <v>26</v>
-      </c>
-      <c r="D58" s="2">
-        <f t="shared" ref="D58" si="30">B58*C58</f>
-        <v>26</v>
-      </c>
-      <c r="E58" s="12">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2">
-        <f t="shared" ref="F58" si="31">D58+E58</f>
-        <v>26</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H58" s="12">
-        <v>1</v>
-      </c>
-      <c r="I58" s="12"/>
-      <c r="J58" s="14">
-        <f t="shared" ref="J58" si="32">F58*H58</f>
-        <v>26</v>
-      </c>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="M58" s="12"/>
-      <c r="N58" s="20"/>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B59" s="12">
-        <v>1</v>
-      </c>
-      <c r="C59" s="21">
-        <v>3</v>
-      </c>
-      <c r="D59" s="2">
-        <f t="shared" ref="D59" si="33">B59*C59</f>
-        <v>3</v>
-      </c>
-      <c r="E59" s="12">
-        <v>0</v>
-      </c>
-      <c r="F59" s="2">
-        <f t="shared" ref="F59" si="34">D59+E59</f>
-        <v>3</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H59" s="12">
-        <v>1</v>
-      </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="14">
-        <f t="shared" ref="J59" si="35">F59*H59</f>
-        <v>3</v>
-      </c>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="M59" s="12"/>
-      <c r="N59" s="20"/>
-    </row>
-    <row r="60" spans="1:15">
-      <c r="A60" s="11"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="20"/>
-    </row>
-    <row r="61" spans="1:15">
-      <c r="A61" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B61" s="12">
-        <v>1</v>
-      </c>
-      <c r="C61" s="21">
-        <v>29.9</v>
-      </c>
-      <c r="D61" s="2">
-        <f t="shared" ref="D61" si="36">B61*C61</f>
-        <v>29.9</v>
-      </c>
-      <c r="E61" s="12">
-        <v>0</v>
-      </c>
-      <c r="F61" s="2">
-        <f t="shared" ref="F61" si="37">D61+E61</f>
-        <v>29.9</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H61" s="12">
-        <v>1</v>
-      </c>
-      <c r="I61" s="12"/>
-      <c r="J61" s="14">
-        <f t="shared" ref="J61" si="38">F61*H61</f>
-        <v>29.9</v>
-      </c>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M61" s="12"/>
-      <c r="N61" s="20"/>
+      <c r="N57" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15" thickBot="1">
+      <c r="A58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="17">
+        <f>SUM(J8:J55)</f>
+        <v>15660.783461999999</v>
+      </c>
+      <c r="K58" s="17">
+        <f>SUM(K8:K55)</f>
+        <v>14513.550000000001</v>
+      </c>
+      <c r="L58" s="17"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="9"/>
     </row>
     <row r="62" spans="1:15">
-      <c r="A62" s="11"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="20"/>
+      <c r="A62" s="24" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="63" spans="1:15">
-      <c r="A63" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="12">
-        <v>2</v>
-      </c>
-      <c r="C63" s="21">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D63" s="2">
-        <f t="shared" si="0"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="E63" s="12">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2">
-        <f t="shared" si="2"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H63" s="12">
-        <v>1</v>
-      </c>
-      <c r="I63" s="12"/>
-      <c r="J63" s="14">
-        <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="N63" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="O63" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
-      <c r="A64" s="11"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="20"/>
-    </row>
-    <row r="65" spans="1:15">
-      <c r="A65" s="11"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="O65" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="15" thickBot="1">
-      <c r="A66" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="17">
-        <f>SUM(J8:J63)</f>
-        <v>16615.813462000002</v>
-      </c>
-      <c r="K66" s="17">
-        <f>SUM(K8:K63)</f>
-        <v>14513.550000000001</v>
-      </c>
-      <c r="L66" s="17"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="9"/>
-    </row>
-    <row r="70" spans="1:15">
-      <c r="A70" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15">
-      <c r="A71" s="25" t="s">
-        <v>142</v>
-      </c>
+      <c r="A63" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>